<commit_message>
dietary index + rewrite hh
in kids module wrote code to compute dietary index
rewrote hh module so now it reads in all variables with Keep=1 in “to
keep” excel spreadsheet automatically
</commit_message>
<xml_diff>
--- a/R/Excel/kids_labels_tokeep.xlsx
+++ b/R/Excel/kids_labels_tokeep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="7600" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="kids_labels_tokeep.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="690">
   <si>
     <t>var</t>
   </si>
@@ -2077,6 +2077,18 @@
   </si>
   <si>
     <t>note: moved from women's module</t>
+  </si>
+  <si>
+    <t>v008</t>
+  </si>
+  <si>
+    <t>date of interview (cmc)</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>interview_date_cmc</t>
   </si>
 </sst>
 </file>
@@ -2456,7 +2468,7 @@
   <dimension ref="A1:G330"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2465,7 +2477,7 @@
     <col min="3" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2481,8 +2493,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>626</v>
       </c>
@@ -2499,7 +2514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2516,7 +2531,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>686</v>
+      </c>
+      <c r="B4" t="s">
+        <v>687</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E4" t="s">
+        <v>644</v>
+      </c>
+      <c r="F4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2533,7 +2568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2550,7 +2585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2567,7 +2602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>411</v>
       </c>
@@ -2584,7 +2619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>412</v>
       </c>
@@ -2601,7 +2636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>414</v>
       </c>
@@ -2618,7 +2653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>416</v>
       </c>
@@ -2635,7 +2670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>418</v>
       </c>
@@ -2652,7 +2687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>420</v>
       </c>
@@ -2669,7 +2704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>424</v>
       </c>
@@ -2686,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>426</v>
       </c>
@@ -2703,7 +2738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>430</v>
       </c>

</xml_diff>